<commit_message>
update shopping malls template for xlsx
</commit_message>
<xml_diff>
--- a/api-service/src/main/resources/docs_templates/template.xlsx
+++ b/api-service/src/main/resources/docs_templates/template.xlsx
@@ -96,9 +96,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -228,16 +232,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>